<commit_message>
fixed native query generation
</commit_message>
<xml_diff>
--- a/datf_core/test/s2t/source_json_target_parquet_s2t_10_mismatch.xlsx
+++ b/datf_core/test/s2t/source_json_target_parquet_s2t_10_mismatch.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TigerAnalytics\accelerator\QE_Automated_Testing_Framework\test\s2t\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Workspaces\GitHub\DATF_Other\Pyspark\QE_ATF\datf_core\test\s2t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97D23AE-231B-4516-B625-D2361A684E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A078CD31-50BE-4CE3-9E30-AFB23371A961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Wk/HSFA0ePxYnHuCg2Xu6V8BJrU2qQuyXxP/xiZ5WP2Fm+GLq8mfRGtBZepFB8vcZ29wwi6DpLHCJ+v9K0Ljbw==" workbookSaltValue="Q4lfZdLtn4rXZBfCNOfu/w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F4CBA58-46F7-48AB-BC01-807547223E03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{1F4CBA58-46F7-48AB-BC01-807547223E03}"/>
   </bookViews>
   <sheets>
     <sheet name="MappingConfiguration" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="129">
   <si>
     <t>mappingname</t>
   </si>
@@ -429,7 +429,7 @@
     <t>/app/test/data/source</t>
   </si>
   <si>
-    <t>/app/test/data/stage</t>
+    <t>/app/test/data/target</t>
   </si>
 </sst>
 </file>
@@ -572,9 +572,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -612,7 +612,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -718,7 +718,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -860,7 +860,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -874,7 +874,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" showOutlineSymbols="0" defaultGridColor="0" colorId="48" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,7 +1085,9 @@
       <c r="A31" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="11"/>
+      <c r="B31" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
@@ -1097,25 +1099,31 @@
       <c r="A33" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="11"/>
+      <c r="B33" s="11" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="11"/>
+      <c r="B34" s="12"/>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="11"/>
+      <c r="B35" s="11" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="11"/>
+      <c r="B36" s="11" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
@@ -1238,8 +1246,8 @@
   </sheetPr>
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" showOutlineSymbols="0" defaultGridColor="0" topLeftCell="A21" colorId="48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:E47"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showOutlineSymbols="0" defaultGridColor="0" colorId="48" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,10 +1738,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>94</v>
@@ -1750,10 +1758,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>95</v>
@@ -1767,10 +1775,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>96</v>
@@ -1784,10 +1792,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>97</v>
@@ -1801,10 +1809,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>98</v>
@@ -1818,10 +1826,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>99</v>
@@ -1835,10 +1840,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>100</v>
@@ -1852,10 +1857,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>101</v>
@@ -1869,10 +1871,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>102</v>
@@ -1886,10 +1888,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>103</v>
@@ -1903,10 +1905,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>104</v>
@@ -1920,10 +1922,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>105</v>
@@ -1937,10 +1939,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>106</v>
@@ -1954,10 +1956,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>107</v>
@@ -1971,10 +1973,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>108</v>
@@ -1988,10 +1990,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>109</v>
@@ -2005,10 +2007,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>110</v>
@@ -2022,10 +2024,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>111</v>
@@ -2039,10 +2041,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>112</v>
@@ -2056,10 +2058,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>113</v>
@@ -2073,10 +2075,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>114</v>
@@ -2090,10 +2092,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>115</v>
@@ -2107,10 +2109,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>116</v>
@@ -2124,10 +2126,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>117</v>
@@ -2141,10 +2143,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>118</v>
@@ -2158,7 +2160,7 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="rOlvHrCO+XNNcwDJkNNMPge1GQY2/YDLQiKdkfA6D+sCe4YvteK2i45uGgCIab6DCLnf4cb3s2h838uqAXzT0w==" saltValue="bUzYlDPS+te7lGdSXPNZxg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576 G1:G1048576 H1:H1048576 I1:I1048576" xr:uid="{928A3064-7F8D-4D02-9A44-B3CAC3FAE93C}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
@@ -2179,7 +2181,7 @@
   <dimension ref="A1:M144"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" showOutlineSymbols="0" defaultGridColor="0" colorId="48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G26"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2854,7 +2856,7 @@
   <dimension ref="A1:P154"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" showOutlineSymbols="0" defaultGridColor="0" colorId="48" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>